<commit_message>
added CFMASO preload, updated some files
</commit_message>
<xml_diff>
--- a/ferric_majorite/autofit/data/this_study_2019-05-03.xlsx
+++ b/ferric_majorite/autofit/data/this_study_2019-05-03.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="220">
   <si>
     <t xml:space="preserve">start mat</t>
   </si>
@@ -640,7 +640,7 @@
     <t xml:space="preserve">ring?</t>
   </si>
   <si>
-    <t xml:space="preserve">fper</t>
+    <t xml:space="preserve">mw</t>
   </si>
   <si>
     <t xml:space="preserve">hpx</t>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t xml:space="preserve">ol</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># The Fe3+/sum(Fe) for the garnet below is a guess based on Z1782 (also Mo-MoO2, KLB-1, 1600C, just 3GPa higher).</t>
   </si>
   <si>
     <t xml:space="preserve">opx</t>
@@ -1027,7 +1030,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1576,6 +1579,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1649,7 +1656,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1895,11 +1902,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48986174"/>
-        <c:axId val="8530602"/>
+        <c:axId val="34034064"/>
+        <c:axId val="16110788"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48986174"/>
+        <c:axId val="34034064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3"/>
@@ -1942,12 +1949,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8530602"/>
+        <c:crossAx val="16110788"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8530602"/>
+        <c:axId val="16110788"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1996,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48986174"/>
+        <c:crossAx val="34034064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2016,7 +2023,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2410,11 +2417,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4666043"/>
-        <c:axId val="44108952"/>
+        <c:axId val="5596976"/>
+        <c:axId val="75406098"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4666043"/>
+        <c:axId val="5596976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -2457,12 +2464,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44108952"/>
+        <c:crossAx val="75406098"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44108952"/>
+        <c:axId val="75406098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2504,7 +2511,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4666043"/>
+        <c:crossAx val="5596976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2531,7 +2538,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2673,11 +2680,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51108688"/>
-        <c:axId val="32604802"/>
+        <c:axId val="53598759"/>
+        <c:axId val="705156"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51108688"/>
+        <c:axId val="53598759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2719,12 +2726,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32604802"/>
+        <c:crossAx val="705156"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32604802"/>
+        <c:axId val="705156"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,7 +2773,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51108688"/>
+        <c:crossAx val="53598759"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2794,7 +2801,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2836,6 +2843,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3096,7 +3104,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.18860970984263</c:v>
+                  <c:v>3.15291874847414</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v/>
@@ -3154,6 +3162,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3418,6 +3427,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3595,6 +3605,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3664,6 +3675,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3703,11 +3715,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48126754"/>
-        <c:axId val="78399621"/>
+        <c:axId val="40007822"/>
+        <c:axId val="18698175"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48126754"/>
+        <c:axId val="40007822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3741,7 +3753,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3763,12 +3775,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78399621"/>
+        <c:crossAx val="18698175"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78399621"/>
+        <c:axId val="18698175"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -3812,7 +3824,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3834,7 +3846,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48126754"/>
+        <c:crossAx val="40007822"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3893,9 +3905,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
+      <xdr:colOff>48600</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3903,8 +3915,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6345000" y="5600520"/>
-        <a:ext cx="6408720" cy="4871520"/>
+        <a:off x="6344280" y="5600520"/>
+        <a:ext cx="6408720" cy="4871160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3923,9 +3935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>58</xdr:col>
-      <xdr:colOff>622440</xdr:colOff>
+      <xdr:colOff>622080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3933,8 +3945,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42500520" y="5756760"/>
-        <a:ext cx="5516280" cy="4901760"/>
+        <a:off x="42490800" y="5756760"/>
+        <a:ext cx="5514120" cy="4901400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3953,9 +3965,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>104400</xdr:colOff>
+      <xdr:colOff>104040</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3963,8 +3975,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="34278120" y="6225480"/>
-        <a:ext cx="7848000" cy="5867280"/>
+        <a:off x="34275600" y="6225480"/>
+        <a:ext cx="7840440" cy="5866920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3988,9 +4000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>175680</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3999,7 +4011,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="54807480" y="4383000"/>
-        <a:ext cx="9657000" cy="5431680"/>
+        <a:ext cx="9656640" cy="5431320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4022,22 +4034,22 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AJ23" activeCellId="0" sqref="AJ23"/>
+      <selection pane="bottomLeft" activeCell="AJ23" activeCellId="1" sqref="B19 AJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="8" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="39" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="39" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="58" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="58" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14393,7 +14405,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="H4" activeCellId="1" sqref="B19 H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38107,10 +38119,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BE1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="BE1" activeCellId="0" sqref="BE1"/>
-      <selection pane="bottomLeft" activeCell="BN16" activeCellId="0" sqref="BN16"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38123,6 +38135,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="87" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="87" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="67" style="87" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="99" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45623,73 +45636,75 @@
       </c>
       <c r="AQ38" s="106" t="e">
         <f aca="false">AP38/(AA38*2 + AC38*1.5 + AE38*(1*(1 - BH38) + 1.5*(BH38)) + AI38 + AK38 + AM38*0.5 + AG38*2 + AO38*2)</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AR38" s="114" t="e">
         <f aca="false">AA38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AS38" s="126" t="e">
         <f aca="false">AB38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AT38" s="126" t="e">
         <f aca="false">AC38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AU38" s="126" t="e">
         <f aca="false">AD38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AV38" s="126" t="e">
         <f aca="false">AE38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AW38" s="126" t="e">
         <f aca="false">AF38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AX38" s="126" t="e">
         <f aca="false">AG38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AY38" s="126" t="e">
         <f aca="false">AH38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AZ38" s="126" t="e">
         <f aca="false">AI38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BA38" s="126" t="e">
         <f aca="false">AJ38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BB38" s="126" t="e">
         <f aca="false">AK38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BC38" s="126" t="e">
         <f aca="false">AL38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BD38" s="126" t="e">
         <f aca="false">AM38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BE38" s="126" t="e">
         <f aca="false">AN38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BF38" s="126" t="e">
         <f aca="false">AO38*$AQ38</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BG38" s="106" t="e">
         <f aca="false">SUM(AR38,AT38,AV38,AX38,AZ38,BB38,BD38,BF38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BH38" s="104"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BH38" s="104" t="s">
+        <v>209</v>
+      </c>
       <c r="BJ38" s="36"/>
       <c r="BK38" s="127"/>
       <c r="BL38" s="127"/>
@@ -45836,31 +45851,31 @@
       </c>
       <c r="AQ39" s="106" t="n">
         <f aca="false">AP39/(AA39*2 + AC39*1.5 + AE39*(1*(1 - BH39) + 1.5*(BH39)) + AI39 + AK39 + AM39*0.5 + AG39*2 + AO39*2)</f>
-        <v>4.19710382160629</v>
+        <v>4.19159421034057</v>
       </c>
       <c r="AR39" s="114" t="n">
         <f aca="false">AA39*$AQ39</f>
-        <v>3.16459392674376</v>
+        <v>3.16043970919487</v>
       </c>
       <c r="AS39" s="126" t="n">
         <f aca="false">AB39*$AQ39</f>
-        <v>0.0977950205003437</v>
+        <v>0.0976666432741465</v>
       </c>
       <c r="AT39" s="126" t="n">
         <f aca="false">AC39*$AQ39</f>
-        <v>1.65480162444658</v>
+        <v>1.6526293375411</v>
       </c>
       <c r="AU39" s="126" t="n">
         <f aca="false">AD39*$AQ39</f>
-        <v>0.164656878054386</v>
+        <v>0.164440730103592</v>
       </c>
       <c r="AV39" s="126" t="n">
         <f aca="false">AE39*$AQ39</f>
-        <v>0.315466296930488</v>
+        <v>0.315052178829674</v>
       </c>
       <c r="AW39" s="126" t="n">
         <f aca="false">AF39*$AQ39</f>
-        <v>0.058419684616757</v>
+        <v>0.0583429960795692</v>
       </c>
       <c r="AX39" s="126" t="n">
         <f aca="false">AG39*$AQ39</f>
@@ -45872,19 +45887,19 @@
       </c>
       <c r="AZ39" s="126" t="n">
         <f aca="false">AI39*$AQ39</f>
-        <v>2.55131061693895</v>
+        <v>2.54796146706921</v>
       </c>
       <c r="BA39" s="126" t="n">
         <f aca="false">AJ39*$AQ39</f>
-        <v>0.104135127221998</v>
+        <v>0.103998427227314</v>
       </c>
       <c r="BB39" s="126" t="n">
         <f aca="false">AK39*$AQ39</f>
-        <v>0.321832795973191</v>
+        <v>0.321410320458232</v>
       </c>
       <c r="BC39" s="126" t="n">
         <f aca="false">AL39*$AQ39</f>
-        <v>0.014968967254567</v>
+        <v>0.0149493172306155</v>
       </c>
       <c r="BD39" s="126" t="n">
         <f aca="false">AM39*$AQ39</f>
@@ -45900,13 +45915,13 @@
       </c>
       <c r="BG39" s="106" t="n">
         <f aca="false">SUM(AR39,AT39,AV39,AX39,AZ39,BB39,BD39,BF39)</f>
-        <v>8.00800526103296</v>
+        <v>7.99749301309309</v>
       </c>
       <c r="BH39" s="104" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="BI39" s="16" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BJ39" s="36" t="str">
         <f aca="false">C39</f>
@@ -45914,11 +45929,11 @@
       </c>
       <c r="BK39" s="127" t="n">
         <f aca="false">AR39</f>
-        <v>3.16459392674376</v>
+        <v>3.16043970919487</v>
       </c>
       <c r="BL39" s="127" t="n">
         <f aca="false">AV39*(1 - BH39) + AZ39+BB39</f>
-        <v>3.18860970984263</v>
+        <v>3.15291874847414</v>
       </c>
       <c r="BM39" s="0"/>
       <c r="BN39" s="127"/>
@@ -46148,7 +46163,7 @@
         <v>175</v>
       </c>
       <c r="B41" s="121" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>56</v>
@@ -48140,7 +48155,7 @@
         <v>157</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>86</v>
@@ -49128,7 +49143,7 @@
         <v>161</v>
       </c>
       <c r="B56" s="75" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>86</v>
@@ -49342,7 +49357,7 @@
         <v>161</v>
       </c>
       <c r="B57" s="121" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>86</v>
@@ -51715,7 +51730,7 @@
         <v>171</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>86</v>
@@ -52511,7 +52526,7 @@
         <v>173</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C73" s="16" t="s">
         <v>86</v>
@@ -52725,7 +52740,7 @@
         <v>173</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C74" s="16" t="s">
         <v>86</v>
@@ -53709,7 +53724,7 @@
         <v>175</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C79" s="16" t="s">
         <v>86</v>
@@ -54700,7 +54715,7 @@
         <v>182</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C84" s="16" t="s">
         <v>86</v>
@@ -55940,7 +55955,7 @@
         <v>163</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>105</v>
@@ -59463,7 +59478,7 @@
         <v>175</v>
       </c>
       <c r="B107" s="87" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C107" s="16" t="s">
         <v>105</v>
@@ -59857,7 +59872,7 @@
         <v>175</v>
       </c>
       <c r="B109" s="87" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>105</v>
@@ -60458,7 +60473,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="1" sqref="B19 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -60471,13 +60486,13 @@
   <sheetData>
     <row r="1" s="135" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="135" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B1" s="135" t="s">
         <v>154</v>
       </c>
       <c r="C1" s="135" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D1" s="135" t="s">
         <v>2</v>
@@ -60489,7 +60504,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="135" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1" s="135" t="s">
         <v>23</v>
@@ -60504,10 +60519,10 @@
         <v>189</v>
       </c>
       <c r="L1" s="135" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M1" s="135" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N1" s="135" t="s">
         <v>65</v>
@@ -60540,10 +60555,10 @@
         <v>18</v>
       </c>
       <c r="X1" s="135" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="Y1" s="135" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -60642,9 +60657,11 @@
         <v>8.0300829394645</v>
       </c>
       <c r="X2" s="87" t="n">
+        <f aca="false">'Model version'!BH3</f>
         <v>0.44</v>
       </c>
       <c r="Y2" s="87" t="n">
+        <f aca="false">'Model version'!BI3</f>
         <v>0.06</v>
       </c>
     </row>
@@ -60741,6 +60758,14 @@
         <f aca="false">SUM(H3,J3,L3,N3,P3,R3,T3,V3)</f>
         <v>2.99799970348482</v>
       </c>
+      <c r="X3" s="87" t="n">
+        <f aca="false">'Model version'!BH4</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="87" t="n">
+        <f aca="false">'Model version'!BI4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="87" t="str">
@@ -60835,6 +60860,14 @@
         <f aca="false">SUM(H4,J4,L4,N4,P4,R4,T4,V4)</f>
         <v>1</v>
       </c>
+      <c r="X4" s="87" t="n">
+        <f aca="false">'Model version'!BH5</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="87" t="n">
+        <f aca="false">'Model version'!BI5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="87" t="str">
@@ -60928,6 +60961,14 @@
       <c r="W5" s="136" t="n">
         <f aca="false">SUM(H5,J5,L5,N5,P5,R5,T5,V5)</f>
         <v>1</v>
+      </c>
+      <c r="X5" s="87" t="n">
+        <f aca="false">'Model version'!BH6</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="87" t="n">
+        <f aca="false">'Model version'!BI6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61042,9 +61083,11 @@
         <v>8.02455919022089</v>
       </c>
       <c r="X7" s="87" t="n">
+        <f aca="false">'Model version'!BH8</f>
         <v>0.47</v>
       </c>
       <c r="Y7" s="87" t="n">
+        <f aca="false">'Model version'!BI8</f>
         <v>0.05</v>
       </c>
     </row>
@@ -61141,6 +61184,14 @@
         <f aca="false">SUM(H8,J8,L8,N8,P8,R8,T8,V8)</f>
         <v>3.00345936566256</v>
       </c>
+      <c r="X8" s="87" t="n">
+        <f aca="false">'Model version'!BH9</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="87" t="n">
+        <f aca="false">'Model version'!BI9</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="87" t="str">
@@ -61235,6 +61286,14 @@
         <f aca="false">SUM(H9,J9,L9,N9,P9,R9,T9,V9)</f>
         <v>1.62508296256645</v>
       </c>
+      <c r="X9" s="87" t="n">
+        <f aca="false">'Model version'!BH10</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="87" t="n">
+        <f aca="false">'Model version'!BI10</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="87" t="str">
@@ -61328,6 +61387,14 @@
       <c r="W10" s="136" t="n">
         <f aca="false">SUM(H10,J10,L10,N10,P10,R10,T10,V10)</f>
         <v>1</v>
+      </c>
+      <c r="X10" s="87" t="n">
+        <f aca="false">'Model version'!BH11</f>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="87" t="n">
+        <f aca="false">'Model version'!BI11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61442,9 +61509,11 @@
         <v>8.05653012347393</v>
       </c>
       <c r="X12" s="87" t="n">
+        <f aca="false">'Model version'!BH13</f>
         <v>0.07</v>
       </c>
       <c r="Y12" s="87" t="n">
+        <f aca="false">'Model version'!BI13</f>
         <v>0.03</v>
       </c>
     </row>
@@ -61541,6 +61610,14 @@
         <f aca="false">SUM(H13,J13,L13,N13,P13,R13,T13,V13)</f>
         <v>3.01596545560866</v>
       </c>
+      <c r="X13" s="87" t="n">
+        <f aca="false">'Model version'!BH14</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="87" t="n">
+        <f aca="false">'Model version'!BI14</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="87" t="str">
@@ -61635,6 +61712,14 @@
         <f aca="false">SUM(H14,J14,L14,N14,P14,R14,T14,V14)</f>
         <v>1</v>
       </c>
+      <c r="X14" s="87" t="n">
+        <f aca="false">'Model version'!BH15</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="87" t="n">
+        <f aca="false">'Model version'!BI15</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="87" t="str">
@@ -61728,6 +61813,14 @@
       <c r="W15" s="136" t="n">
         <f aca="false">SUM(H15,J15,L15,N15,P15,R15,T15,V15)</f>
         <v>1</v>
+      </c>
+      <c r="X15" s="87" t="n">
+        <f aca="false">'Model version'!BH16</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="87" t="n">
+        <f aca="false">'Model version'!BI16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61842,9 +61935,11 @@
         <v>8.05949510114354</v>
       </c>
       <c r="X17" s="87" t="n">
+        <f aca="false">'Model version'!BH18</f>
         <v>0.09</v>
       </c>
       <c r="Y17" s="87" t="n">
+        <f aca="false">'Model version'!BI18</f>
         <v>0.04</v>
       </c>
     </row>
@@ -61855,7 +61950,7 @@
       </c>
       <c r="B18" s="87" t="str">
         <f aca="false">'Model version'!B19</f>
-        <v>fper</v>
+        <v>mw</v>
       </c>
       <c r="C18" s="87" t="str">
         <f aca="false">'Model version'!C19</f>
@@ -61940,6 +62035,14 @@
       <c r="W18" s="136" t="n">
         <f aca="false">SUM(H18,J18,L18,N18,P18,R18,T18,V18)</f>
         <v>1.99783929794862</v>
+      </c>
+      <c r="X18" s="87" t="n">
+        <f aca="false">'Model version'!BH19</f>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="87" t="n">
+        <f aca="false">'Model version'!BI19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62035,6 +62138,14 @@
         <f aca="false">SUM(H19,J19,L19,N19,P19,R19,T19,V19)</f>
         <v>3.00209729639035</v>
       </c>
+      <c r="X19" s="87" t="n">
+        <f aca="false">'Model version'!BH20</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="87" t="n">
+        <f aca="false">'Model version'!BI20</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="87" t="str">
@@ -62129,6 +62240,14 @@
         <f aca="false">SUM(H20,J20,L20,N20,P20,R20,T20,V20)</f>
         <v>4.00678351764766</v>
       </c>
+      <c r="X20" s="87" t="n">
+        <f aca="false">'Model version'!BH21</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="87" t="n">
+        <f aca="false">'Model version'!BI21</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="87" t="str">
@@ -62222,6 +62341,14 @@
       <c r="W21" s="136" t="n">
         <f aca="false">SUM(H21,J21,L21,N21,P21,R21,T21,V21)</f>
         <v>1</v>
+      </c>
+      <c r="X21" s="87" t="n">
+        <f aca="false">'Model version'!BH22</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="87" t="n">
+        <f aca="false">'Model version'!BI22</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62336,9 +62463,11 @@
         <v>8.01012014762233</v>
       </c>
       <c r="X23" s="87" t="n">
+        <f aca="false">'Model version'!BH24</f>
         <v>0.08</v>
       </c>
       <c r="Y23" s="87" t="n">
+        <f aca="false">'Model version'!BI24</f>
         <v>0.03</v>
       </c>
     </row>
@@ -62435,6 +62564,14 @@
         <f aca="false">SUM(H24,J24,L24,N24,P24,R24,T24,V24)</f>
         <v>2.99043024806282</v>
       </c>
+      <c r="X24" s="87" t="n">
+        <f aca="false">'Model version'!BH25</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="87" t="n">
+        <f aca="false">'Model version'!BI25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="87" t="str">
@@ -62529,6 +62666,14 @@
         <f aca="false">SUM(H25,J25,L25,N25,P25,R25,T25,V25)</f>
         <v>3.99136621986675</v>
       </c>
+      <c r="X25" s="87" t="n">
+        <f aca="false">'Model version'!BH26</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="87" t="n">
+        <f aca="false">'Model version'!BI26</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="87" t="str">
@@ -62623,6 +62768,14 @@
         <f aca="false">SUM(H26,J26,L26,N26,P26,R26,T26,V26)</f>
         <v>1</v>
       </c>
+      <c r="X26" s="87" t="n">
+        <f aca="false">'Model version'!BH27</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="87" t="n">
+        <f aca="false">'Model version'!BI27</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="87" t="str">
@@ -62716,6 +62869,14 @@
       <c r="W27" s="136" t="n">
         <f aca="false">SUM(H27,J27,L27,N27,P27,R27,T27,V27)</f>
         <v>1</v>
+      </c>
+      <c r="X27" s="87" t="n">
+        <f aca="false">'Model version'!BH28</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="87" t="n">
+        <f aca="false">'Model version'!BI28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -62830,9 +62991,11 @@
         <v>8.01346450775364</v>
       </c>
       <c r="X29" s="87" t="n">
+        <f aca="false">'Model version'!BH30</f>
         <v>0.14</v>
       </c>
       <c r="Y29" s="87" t="n">
+        <f aca="false">'Model version'!BI30</f>
         <v>0.04</v>
       </c>
     </row>
@@ -62929,6 +63092,14 @@
         <f aca="false">SUM(H30,J30,L30,N30,P30,R30,T30,V30)</f>
         <v>3.00932455561492</v>
       </c>
+      <c r="X30" s="87" t="n">
+        <f aca="false">'Model version'!BH31</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="87" t="n">
+        <f aca="false">'Model version'!BI31</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="87" t="str">
@@ -63022,6 +63193,14 @@
       <c r="W31" s="136" t="n">
         <f aca="false">SUM(H31,J31,L31,N31,P31,R31,T31,V31)</f>
         <v>1</v>
+      </c>
+      <c r="X31" s="87" t="n">
+        <f aca="false">'Model version'!BH32</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="87" t="n">
+        <f aca="false">'Model version'!BI32</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63136,9 +63315,11 @@
         <v>8.04406488720404</v>
       </c>
       <c r="X33" s="87" t="n">
+        <f aca="false">'Model version'!BH34</f>
         <v>0.29</v>
       </c>
       <c r="Y33" s="87" t="n">
+        <f aca="false">'Model version'!BI34</f>
         <v>0.04</v>
       </c>
     </row>
@@ -63235,6 +63416,14 @@
         <f aca="false">SUM(H34,J34,L34,N34,P34,R34,T34,V34)</f>
         <v>3.0083565570347</v>
       </c>
+      <c r="X34" s="87" t="n">
+        <f aca="false">'Model version'!BH35</f>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="87" t="n">
+        <f aca="false">'Model version'!BI35</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="87" t="str">
@@ -63329,6 +63518,14 @@
         <f aca="false">SUM(H35,J35,L35,N35,P35,R35,T35,V35)</f>
         <v>1</v>
       </c>
+      <c r="X35" s="87" t="n">
+        <f aca="false">'Model version'!BH36</f>
+        <v>0</v>
+      </c>
+      <c r="Y35" s="87" t="n">
+        <f aca="false">'Model version'!BI36</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="87" t="str">
@@ -63423,8 +63620,20 @@
         <f aca="false">SUM(H36,J36,L36,N36,P36,R36,T36,V36)</f>
         <v>1</v>
       </c>
+      <c r="X36" s="87" t="n">
+        <f aca="false">'Model version'!BH37</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="87" t="n">
+        <f aca="false">'Model version'!BI37</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="87" t="str">
+        <f aca="false">'Model version'!BH38</f>
+        <v># The Fe3+/sum(Fe) for the garnet below is a guess based on Z1782 (also Mo-MoO2, KLB-1, 1600C, just 3GPa higher).</v>
+      </c>
       <c r="H37" s="136"/>
       <c r="I37" s="136"/>
       <c r="J37" s="136"/>
@@ -63441,6 +63650,7 @@
       <c r="U37" s="136"/>
       <c r="V37" s="136"/>
       <c r="W37" s="136"/>
+      <c r="X37" s="137"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="87" t="str">
@@ -63473,27 +63683,27 @@
       </c>
       <c r="H38" s="136" t="n">
         <f aca="false">'Model version'!AR39</f>
-        <v>3.16459392674376</v>
+        <v>3.16043970919487</v>
       </c>
       <c r="I38" s="136" t="n">
         <f aca="false">'Model version'!AS39</f>
-        <v>0.0977950205003437</v>
+        <v>0.0976666432741465</v>
       </c>
       <c r="J38" s="136" t="n">
         <f aca="false">'Model version'!AT39</f>
-        <v>1.65480162444658</v>
+        <v>1.6526293375411</v>
       </c>
       <c r="K38" s="136" t="n">
         <f aca="false">'Model version'!AU39</f>
-        <v>0.164656878054386</v>
+        <v>0.164440730103592</v>
       </c>
       <c r="L38" s="136" t="n">
         <f aca="false">'Model version'!AV39</f>
-        <v>0.315466296930488</v>
+        <v>0.315052178829674</v>
       </c>
       <c r="M38" s="136" t="n">
         <f aca="false">'Model version'!AW39</f>
-        <v>0.058419684616757</v>
+        <v>0.0583429960795692</v>
       </c>
       <c r="N38" s="136" t="n">
         <f aca="false">'Model version'!AX39</f>
@@ -63505,19 +63715,19 @@
       </c>
       <c r="P38" s="136" t="n">
         <f aca="false">'Model version'!AZ39</f>
-        <v>2.55131061693895</v>
+        <v>2.54796146706921</v>
       </c>
       <c r="Q38" s="136" t="n">
         <f aca="false">'Model version'!BA39</f>
-        <v>0.104135127221998</v>
+        <v>0.103998427227314</v>
       </c>
       <c r="R38" s="136" t="n">
         <f aca="false">'Model version'!BB39</f>
-        <v>0.321832795973191</v>
+        <v>0.321410320458232</v>
       </c>
       <c r="S38" s="136" t="n">
         <f aca="false">'Model version'!BC39</f>
-        <v>0.014968967254567</v>
+        <v>0.0149493172306155</v>
       </c>
       <c r="T38" s="136" t="n">
         <f aca="false">'Model version'!BD39</f>
@@ -63533,13 +63743,15 @@
       </c>
       <c r="W38" s="136" t="n">
         <f aca="false">SUM(H38,J38,L38,N38,P38,R38,T38,V38)</f>
-        <v>8.00800526103296</v>
+        <v>7.99749301309309</v>
       </c>
       <c r="X38" s="87" t="n">
-        <v>0</v>
+        <f aca="false">'Model version'!BH39</f>
+        <v>0.1</v>
       </c>
       <c r="Y38" s="87" t="n">
-        <v>0</v>
+        <f aca="false">'Model version'!BI39</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63635,6 +63847,14 @@
         <f aca="false">SUM(H39,J39,L39,N39,P39,R39,T39,V39)</f>
         <v>2.99400443280718</v>
       </c>
+      <c r="X39" s="87" t="n">
+        <f aca="false">'Model version'!BH40</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="87" t="n">
+        <f aca="false">'Model version'!BI40</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="87" t="str">
@@ -63729,6 +63949,14 @@
         <f aca="false">SUM(H40,J40,L40,N40,P40,R40,T40,V40)</f>
         <v>3.99034904341379</v>
       </c>
+      <c r="X40" s="87" t="n">
+        <f aca="false">'Model version'!BH41</f>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="87" t="n">
+        <f aca="false">'Model version'!BI41</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="87" t="str">
@@ -63823,6 +64051,14 @@
         <f aca="false">SUM(H41,J41,L41,N41,P41,R41,T41,V41)</f>
         <v>1</v>
       </c>
+      <c r="X41" s="87" t="n">
+        <f aca="false">'Model version'!BH42</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="87" t="n">
+        <f aca="false">'Model version'!BI42</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="87" t="str">
@@ -63916,6 +64152,14 @@
       <c r="W42" s="136" t="n">
         <f aca="false">SUM(H42,J42,L42,N42,P42,R42,T42,V42)</f>
         <v>1</v>
+      </c>
+      <c r="X42" s="87" t="n">
+        <f aca="false">'Model version'!BH43</f>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="87" t="n">
+        <f aca="false">'Model version'!BI43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64030,9 +64274,11 @@
         <v>8.02564179961104</v>
       </c>
       <c r="X44" s="87" t="n">
+        <f aca="false">'Model version'!BH45</f>
         <v>0.14</v>
       </c>
       <c r="Y44" s="87" t="n">
+        <f aca="false">'Model version'!BI45</f>
         <v>0.04</v>
       </c>
     </row>
@@ -64129,6 +64375,14 @@
         <f aca="false">SUM(H45,J45,L45,N45,P45,R45,T45,V45)</f>
         <v>2.99165698273696</v>
       </c>
+      <c r="X45" s="87" t="n">
+        <f aca="false">'Model version'!BH46</f>
+        <v>0</v>
+      </c>
+      <c r="Y45" s="87" t="n">
+        <f aca="false">'Model version'!BI46</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="87" t="str">
@@ -64222,6 +64476,14 @@
       <c r="W46" s="136" t="n">
         <f aca="false">SUM(H46,J46,L46,N46,P46,R46,T46,V46)</f>
         <v>1</v>
+      </c>
+      <c r="X46" s="87" t="n">
+        <f aca="false">'Model version'!BH47</f>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="87" t="n">
+        <f aca="false">'Model version'!BI47</f>
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64354,9 +64616,11 @@
         <v>8.00548271681929</v>
       </c>
       <c r="X49" s="87" t="n">
+        <f aca="false">'Model version'!BH50</f>
         <v>0.21</v>
       </c>
       <c r="Y49" s="87" t="n">
+        <f aca="false">'Model version'!BI50</f>
         <v>0.03</v>
       </c>
     </row>
@@ -64453,6 +64717,14 @@
         <f aca="false">SUM(H50,J50,L50,N50,P50,R50,T50,V50)</f>
         <v>1.00772296192501</v>
       </c>
+      <c r="X50" s="87" t="n">
+        <f aca="false">'Model version'!BH51</f>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="87" t="n">
+        <f aca="false">'Model version'!BI51</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="87" t="str">
@@ -64547,6 +64819,14 @@
         <f aca="false">SUM(H51,J51,L51,N51,P51,R51,T51,V51)</f>
         <v>1</v>
       </c>
+      <c r="X51" s="87" t="n">
+        <f aca="false">'Model version'!BH52</f>
+        <v>0</v>
+      </c>
+      <c r="Y51" s="87" t="n">
+        <f aca="false">'Model version'!BI52</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="87" t="str">
@@ -64640,6 +64920,14 @@
       <c r="W52" s="136" t="n">
         <f aca="false">SUM(H52,J52,L52,N52,P52,R52,T52,V52)</f>
         <v>1</v>
+      </c>
+      <c r="X52" s="87" t="n">
+        <f aca="false">'Model version'!BH53</f>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="87" t="n">
+        <f aca="false">'Model version'!BI53</f>
+        <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -64754,9 +65042,11 @@
         <v>7.99125655605406</v>
       </c>
       <c r="X54" s="87" t="n">
+        <f aca="false">'Model version'!BH55</f>
         <v>0.15</v>
       </c>
       <c r="Y54" s="87" t="n">
+        <f aca="false">'Model version'!BI55</f>
         <v>0.02</v>
       </c>
     </row>
@@ -64853,6 +65143,14 @@
         <f aca="false">SUM(H55,J55,L55,N55,P55,R55,T55,V55)</f>
         <v>3.97671428020264</v>
       </c>
+      <c r="X55" s="87" t="n">
+        <f aca="false">'Model version'!BH56</f>
+        <v>0</v>
+      </c>
+      <c r="Y55" s="87" t="n">
+        <f aca="false">'Model version'!BI56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="87" t="str">
@@ -64947,6 +65245,14 @@
         <f aca="false">SUM(H56,J56,L56,N56,P56,R56,T56,V56)</f>
         <v>1.00590622394891</v>
       </c>
+      <c r="X56" s="87" t="n">
+        <f aca="false">'Model version'!BH57</f>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="87" t="n">
+        <f aca="false">'Model version'!BI57</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="87" t="str">
@@ -65041,6 +65347,14 @@
         <f aca="false">SUM(H57,J57,L57,N57,P57,R57,T57,V57)</f>
         <v>1</v>
       </c>
+      <c r="X57" s="87" t="n">
+        <f aca="false">'Model version'!BH58</f>
+        <v>0</v>
+      </c>
+      <c r="Y57" s="87" t="n">
+        <f aca="false">'Model version'!BI58</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="87" t="str">
@@ -65134,6 +65448,14 @@
       <c r="W58" s="136" t="n">
         <f aca="false">SUM(H58,J58,L58,N58,P58,R58,T58,V58)</f>
         <v>1</v>
+      </c>
+      <c r="X58" s="87" t="n">
+        <f aca="false">'Model version'!BH59</f>
+        <v>0</v>
+      </c>
+      <c r="Y58" s="87" t="n">
+        <f aca="false">'Model version'!BI59</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65248,9 +65570,11 @@
         <v>7.75509695717206</v>
       </c>
       <c r="X60" s="87" t="n">
+        <f aca="false">'Model version'!BH61</f>
         <v>0.08</v>
       </c>
       <c r="Y60" s="87" t="n">
+        <f aca="false">'Model version'!BI61</f>
         <v>0.04</v>
       </c>
     </row>
@@ -65347,6 +65671,14 @@
         <f aca="false">SUM(H61,J61,L61,N61,P61,R61,T61,V61)</f>
         <v>0.5</v>
       </c>
+      <c r="X61" s="87" t="n">
+        <f aca="false">'Model version'!BH62</f>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="87" t="n">
+        <f aca="false">'Model version'!BI62</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="87" t="str">
@@ -65440,6 +65772,14 @@
       <c r="W62" s="136" t="n">
         <f aca="false">SUM(H62,J62,L62,N62,P62,R62,T62,V62)</f>
         <v>1</v>
+      </c>
+      <c r="X62" s="87" t="n">
+        <f aca="false">'Model version'!BH63</f>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="87" t="n">
+        <f aca="false">'Model version'!BI63</f>
+        <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65554,9 +65894,11 @@
         <v>7.82471857660023</v>
       </c>
       <c r="X64" s="87" t="n">
+        <f aca="false">'Model version'!BH65</f>
         <v>0.11</v>
       </c>
       <c r="Y64" s="87" t="n">
+        <f aca="false">'Model version'!BI65</f>
         <v>0.06</v>
       </c>
     </row>
@@ -65652,6 +65994,14 @@
       <c r="W65" s="136" t="n">
         <f aca="false">SUM(H65,J65,L65,N65,P65,R65,T65,V65)</f>
         <v>1</v>
+      </c>
+      <c r="X65" s="87" t="n">
+        <f aca="false">'Model version'!BH66</f>
+        <v>0</v>
+      </c>
+      <c r="Y65" s="87" t="n">
+        <f aca="false">'Model version'!BI66</f>
+        <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65766,9 +66116,11 @@
         <v>7.93966407109845</v>
       </c>
       <c r="X67" s="87" t="n">
+        <f aca="false">'Model version'!BH68</f>
         <v>0.03</v>
       </c>
       <c r="Y67" s="87" t="n">
+        <f aca="false">'Model version'!BI68</f>
         <v>0.01</v>
       </c>
     </row>
@@ -65865,6 +66217,14 @@
         <f aca="false">SUM(H68,J68,L68,N68,P68,R68,T68,V68)</f>
         <v>3.98495340987772</v>
       </c>
+      <c r="X68" s="87" t="n">
+        <f aca="false">'Model version'!BH69</f>
+        <v>0</v>
+      </c>
+      <c r="Y68" s="87" t="n">
+        <f aca="false">'Model version'!BI69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="87" t="str">
@@ -65958,6 +66318,14 @@
       <c r="W69" s="136" t="n">
         <f aca="false">SUM(H69,J69,L69,N69,P69,R69,T69,V69)</f>
         <v>1</v>
+      </c>
+      <c r="X69" s="87" t="n">
+        <f aca="false">'Model version'!BH70</f>
+        <v>0</v>
+      </c>
+      <c r="Y69" s="87" t="n">
+        <f aca="false">'Model version'!BI70</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66072,9 +66440,11 @@
         <v>7.96693841168912</v>
       </c>
       <c r="X71" s="87" t="n">
+        <f aca="false">'Model version'!BH72</f>
         <v>0.23</v>
       </c>
       <c r="Y71" s="87" t="n">
+        <f aca="false">'Model version'!BI72</f>
         <v>0.03</v>
       </c>
     </row>
@@ -66171,6 +66541,14 @@
         <f aca="false">SUM(H72,J72,L72,N72,P72,R72,T72,V72)</f>
         <v>3.95326905456945</v>
       </c>
+      <c r="X72" s="87" t="n">
+        <f aca="false">'Model version'!BH73</f>
+        <v>0</v>
+      </c>
+      <c r="Y72" s="87" t="n">
+        <f aca="false">'Model version'!BI73</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="87" t="str">
@@ -66265,6 +66643,14 @@
         <f aca="false">SUM(H73,J73,L73,N73,P73,R73,T73,V73)</f>
         <v>1.00186713720383</v>
       </c>
+      <c r="X73" s="87" t="n">
+        <f aca="false">'Model version'!BH74</f>
+        <v>0</v>
+      </c>
+      <c r="Y73" s="87" t="n">
+        <f aca="false">'Model version'!BI74</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="87" t="str">
@@ -66359,6 +66745,14 @@
         <f aca="false">SUM(H74,J74,L74,N74,P74,R74,T74,V74)</f>
         <v>1</v>
       </c>
+      <c r="X74" s="87" t="n">
+        <f aca="false">'Model version'!BH75</f>
+        <v>0</v>
+      </c>
+      <c r="Y74" s="87" t="n">
+        <f aca="false">'Model version'!BI75</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="87" t="str">
@@ -66452,6 +66846,14 @@
       <c r="W75" s="136" t="n">
         <f aca="false">SUM(H75,J75,L75,N75,P75,R75,T75,V75)</f>
         <v>1</v>
+      </c>
+      <c r="X75" s="87" t="n">
+        <f aca="false">'Model version'!BH76</f>
+        <v>0</v>
+      </c>
+      <c r="Y75" s="87" t="n">
+        <f aca="false">'Model version'!BI76</f>
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66566,9 +66968,11 @@
         <v>7.98782390877014</v>
       </c>
       <c r="X77" s="87" t="n">
+        <f aca="false">'Model version'!BH78</f>
         <v>0.21</v>
       </c>
       <c r="Y77" s="87" t="n">
+        <f aca="false">'Model version'!BI78</f>
         <v>0.02</v>
       </c>
     </row>
@@ -66665,6 +67069,14 @@
         <f aca="false">SUM(H78,J78,L78,N78,P78,R78,T78,V78)</f>
         <v>3.99230426574325</v>
       </c>
+      <c r="X78" s="87" t="n">
+        <f aca="false">'Model version'!BH79</f>
+        <v>0</v>
+      </c>
+      <c r="Y78" s="87" t="n">
+        <f aca="false">'Model version'!BI79</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="87" t="str">
@@ -66759,6 +67171,14 @@
         <f aca="false">SUM(H79,J79,L79,N79,P79,R79,T79,V79)</f>
         <v>0.5</v>
       </c>
+      <c r="X79" s="87" t="n">
+        <f aca="false">'Model version'!BH80</f>
+        <v>0</v>
+      </c>
+      <c r="Y79" s="87" t="n">
+        <f aca="false">'Model version'!BI80</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="87" t="str">
@@ -66852,6 +67272,14 @@
       <c r="W80" s="136" t="n">
         <f aca="false">SUM(H80,J80,L80,N80,P80,R80,T80,V80)</f>
         <v>1</v>
+      </c>
+      <c r="X80" s="87" t="n">
+        <f aca="false">'Model version'!BH81</f>
+        <v>0</v>
+      </c>
+      <c r="Y80" s="87" t="n">
+        <f aca="false">'Model version'!BI81</f>
+        <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66966,9 +67394,11 @@
         <v>7.97643826506405</v>
       </c>
       <c r="X82" s="87" t="n">
+        <f aca="false">'Model version'!BH83</f>
         <v>0.09</v>
       </c>
       <c r="Y82" s="87" t="n">
+        <f aca="false">'Model version'!BI83</f>
         <v>0.02</v>
       </c>
     </row>
@@ -67065,6 +67495,14 @@
         <f aca="false">SUM(H83,J83,L83,N83,P83,R83,T83,V83)</f>
         <v>3.977970294945</v>
       </c>
+      <c r="X83" s="87" t="n">
+        <f aca="false">'Model version'!BH84</f>
+        <v>0</v>
+      </c>
+      <c r="Y83" s="87" t="n">
+        <f aca="false">'Model version'!BI84</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="87" t="str">
@@ -67158,6 +67596,14 @@
       <c r="W84" s="136" t="n">
         <f aca="false">SUM(H84,J84,L84,N84,P84,R84,T84,V84)</f>
         <v>1</v>
+      </c>
+      <c r="X84" s="87" t="n">
+        <f aca="false">'Model version'!BH85</f>
+        <v>0</v>
+      </c>
+      <c r="Y84" s="87" t="n">
+        <f aca="false">'Model version'!BI85</f>
+        <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67272,9 +67718,11 @@
         <v>8.06576993251338</v>
       </c>
       <c r="X86" s="87" t="n">
+        <f aca="false">'Model version'!BH87</f>
         <v>0.05</v>
       </c>
       <c r="Y86" s="87" t="n">
+        <f aca="false">'Model version'!BI87</f>
         <v>0.02</v>
       </c>
     </row>
@@ -67371,6 +67819,14 @@
         <f aca="false">SUM(H87,J87,L87,N87,P87,R87,T87,V87)</f>
         <v>3.01667258801356</v>
       </c>
+      <c r="X87" s="87" t="n">
+        <f aca="false">'Model version'!BH88</f>
+        <v>0</v>
+      </c>
+      <c r="Y87" s="87" t="n">
+        <f aca="false">'Model version'!BI88</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="87" t="str">
@@ -67465,6 +67921,14 @@
         <f aca="false">SUM(H88,J88,L88,N88,P88,R88,T88,V88)</f>
         <v>4.0221699747513</v>
       </c>
+      <c r="X88" s="87" t="n">
+        <f aca="false">'Model version'!BH89</f>
+        <v>0</v>
+      </c>
+      <c r="Y88" s="87" t="n">
+        <f aca="false">'Model version'!BI89</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="87" t="str">
@@ -67559,6 +68023,14 @@
         <f aca="false">SUM(H89,J89,L89,N89,P89,R89,T89,V89)</f>
         <v>1.00482830731852</v>
       </c>
+      <c r="X89" s="87" t="n">
+        <f aca="false">'Model version'!BH90</f>
+        <v>0</v>
+      </c>
+      <c r="Y89" s="87" t="n">
+        <f aca="false">'Model version'!BI90</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="87" t="str">
@@ -67653,6 +68125,14 @@
         <f aca="false">SUM(H90,J90,L90,N90,P90,R90,T90,V90)</f>
         <v>1</v>
       </c>
+      <c r="X90" s="87" t="n">
+        <f aca="false">'Model version'!BH91</f>
+        <v>0</v>
+      </c>
+      <c r="Y90" s="87" t="n">
+        <f aca="false">'Model version'!BI91</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="87" t="str">
@@ -67746,6 +68226,14 @@
       <c r="W91" s="136" t="n">
         <f aca="false">SUM(H91,J91,L91,N91,P91,R91,T91,V91)</f>
         <v>1</v>
+      </c>
+      <c r="X91" s="87" t="n">
+        <f aca="false">'Model version'!BH92</f>
+        <v>0</v>
+      </c>
+      <c r="Y91" s="87" t="n">
+        <f aca="false">'Model version'!BI92</f>
+        <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -67860,9 +68348,11 @@
         <v>8.04753049285862</v>
       </c>
       <c r="X93" s="87" t="n">
+        <f aca="false">'Model version'!BH94</f>
         <v>0.08</v>
       </c>
       <c r="Y93" s="87" t="n">
+        <f aca="false">'Model version'!BI94</f>
         <v>0.02</v>
       </c>
     </row>
@@ -67959,6 +68449,14 @@
         <f aca="false">SUM(H94,J94,L94,N94,P94,R94,T94,V94)</f>
         <v>3.01503276800036</v>
       </c>
+      <c r="X94" s="87" t="n">
+        <f aca="false">'Model version'!BH95</f>
+        <v>0</v>
+      </c>
+      <c r="Y94" s="87" t="n">
+        <f aca="false">'Model version'!BI95</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="87" t="str">
@@ -68053,6 +68551,14 @@
         <f aca="false">SUM(H95,J95,L95,N95,P95,R95,T95,V95)</f>
         <v>2.99778708130697</v>
       </c>
+      <c r="X95" s="87" t="n">
+        <f aca="false">'Model version'!BH96</f>
+        <v>0</v>
+      </c>
+      <c r="Y95" s="87" t="n">
+        <f aca="false">'Model version'!BI96</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="87" t="str">
@@ -68146,6 +68652,14 @@
       <c r="W96" s="136" t="n">
         <f aca="false">SUM(H96,J96,L96,N96,P96,R96,T96,V96)</f>
         <v>1</v>
+      </c>
+      <c r="X96" s="87" t="n">
+        <f aca="false">'Model version'!BH97</f>
+        <v>0</v>
+      </c>
+      <c r="Y96" s="87" t="n">
+        <f aca="false">'Model version'!BI97</f>
+        <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68260,9 +68774,11 @@
         <v>7.99735021723903</v>
       </c>
       <c r="X98" s="87" t="n">
+        <f aca="false">'Model version'!BH99</f>
         <v>0.1</v>
       </c>
       <c r="Y98" s="87" t="n">
+        <f aca="false">'Model version'!BI99</f>
         <v>0.04</v>
       </c>
     </row>
@@ -68359,6 +68875,14 @@
         <f aca="false">SUM(H99,J99,L99,N99,P99,R99,T99,V99)</f>
         <v>2.99869619389482</v>
       </c>
+      <c r="X99" s="87" t="n">
+        <f aca="false">'Model version'!BH100</f>
+        <v>0</v>
+      </c>
+      <c r="Y99" s="87" t="n">
+        <f aca="false">'Model version'!BI100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="87" t="str">
@@ -68453,6 +68977,14 @@
         <f aca="false">SUM(H100,J100,L100,N100,P100,R100,T100,V100)</f>
         <v>3.00087379017567</v>
       </c>
+      <c r="X100" s="87" t="n">
+        <f aca="false">'Model version'!BH101</f>
+        <v>0</v>
+      </c>
+      <c r="Y100" s="87" t="n">
+        <f aca="false">'Model version'!BI101</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="87" t="str">
@@ -68547,6 +69079,14 @@
         <f aca="false">SUM(H101,J101,L101,N101,P101,R101,T101,V101)</f>
         <v>3.996338118476</v>
       </c>
+      <c r="X101" s="87" t="n">
+        <f aca="false">'Model version'!BH102</f>
+        <v>0</v>
+      </c>
+      <c r="Y101" s="87" t="n">
+        <f aca="false">'Model version'!BI102</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="87" t="str">
@@ -68641,6 +69181,14 @@
         <f aca="false">SUM(H102,J102,L102,N102,P102,R102,T102,V102)</f>
         <v>1</v>
       </c>
+      <c r="X102" s="87" t="n">
+        <f aca="false">'Model version'!BH103</f>
+        <v>0</v>
+      </c>
+      <c r="Y102" s="87" t="n">
+        <f aca="false">'Model version'!BI103</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="87" t="str">
@@ -68734,6 +69282,14 @@
       <c r="W103" s="136" t="n">
         <f aca="false">SUM(H103,J103,L103,N103,P103,R103,T103,V103)</f>
         <v>1</v>
+      </c>
+      <c r="X103" s="87" t="n">
+        <f aca="false">'Model version'!BH104</f>
+        <v>0</v>
+      </c>
+      <c r="Y103" s="87" t="n">
+        <f aca="false">'Model version'!BI104</f>
+        <v>0</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68848,9 +69404,11 @@
         <v>8.03741637970117</v>
       </c>
       <c r="X105" s="87" t="n">
+        <f aca="false">'Model version'!BH106</f>
         <v>0.16</v>
       </c>
       <c r="Y105" s="87" t="n">
+        <f aca="false">'Model version'!BI106</f>
         <v>0.03</v>
       </c>
     </row>
@@ -68947,6 +69505,14 @@
         <f aca="false">SUM(H106,J106,L106,N106,P106,R106,T106,V106)</f>
         <v>4.02160882077545</v>
       </c>
+      <c r="X106" s="87" t="n">
+        <f aca="false">'Model version'!BH107</f>
+        <v>0</v>
+      </c>
+      <c r="Y106" s="87" t="n">
+        <f aca="false">'Model version'!BI107</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="87" t="str">
@@ -69041,6 +69607,14 @@
         <f aca="false">SUM(H107,J107,L107,N107,P107,R107,T107,V107)</f>
         <v>3.02405941445425</v>
       </c>
+      <c r="X107" s="87" t="n">
+        <f aca="false">'Model version'!BH108</f>
+        <v>0</v>
+      </c>
+      <c r="Y107" s="87" t="n">
+        <f aca="false">'Model version'!BI108</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="87" t="str">
@@ -69135,6 +69709,14 @@
         <f aca="false">SUM(H108,J108,L108,N108,P108,R108,T108,V108)</f>
         <v>4.0360979097926</v>
       </c>
+      <c r="X108" s="87" t="n">
+        <f aca="false">'Model version'!BH109</f>
+        <v>0</v>
+      </c>
+      <c r="Y108" s="87" t="n">
+        <f aca="false">'Model version'!BI109</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="87" t="str">
@@ -69229,6 +69811,14 @@
         <f aca="false">SUM(H109,J109,L109,N109,P109,R109,T109,V109)</f>
         <v>1</v>
       </c>
+      <c r="X109" s="87" t="n">
+        <f aca="false">'Model version'!BH110</f>
+        <v>0</v>
+      </c>
+      <c r="Y109" s="87" t="n">
+        <f aca="false">'Model version'!BI110</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="87" t="str">
@@ -69322,6 +69912,14 @@
       <c r="W110" s="136" t="n">
         <f aca="false">SUM(H110,J110,L110,N110,P110,R110,T110,V110)</f>
         <v>1</v>
+      </c>
+      <c r="X110" s="87" t="n">
+        <f aca="false">'Model version'!BH111</f>
+        <v>0</v>
+      </c>
+      <c r="Y110" s="87" t="n">
+        <f aca="false">'Model version'!BI111</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>